<commit_message>
fix: corrected wrong dates in journal and summary tables
</commit_message>
<xml_diff>
--- a/profiles/standard/documents/journal.xlsx
+++ b/profiles/standard/documents/journal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\isaba6\git\llm-aicc-testbot\profiles\anamnes\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\isaba6\git\vitalis-demo\profiles\standard\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF8B4CB-697A-4E05-A032-3E25AAB436CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEA2E8E-C3EA-46E9-967A-0CD8EF4F82CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,16 +100,6 @@
     <t>Operationsberättelse</t>
   </si>
   <si>
-    <t>Operationsberättelse 24-01-25, kl 0123, Läk Robin Gyllenskjöld: 
-Operationskod: AAD10 Utrymning av kroniskt subduralthematom höger
-Operatör: Robin Gyllenskjöld
-Operation: 5 Sahlgrenska
-Preoperativ bedömning: 63 årig man med HT, HL, rökare, som för ca 1 månad sedan ramlade och slog i huvudet. För ca 1 vecka sedan utvecklat smygande vä svaghet, haltande vä ben vid gång, balansbesvär, konstant tryckande huvudvärk VAS 6-7, förvirring. Inneliggande sedan igår 23-01-23. Under kvällen kliniskt försämrad, RLS 2-3, ytterligare vä svaghet. Bedöms indikation för akut utrymning. 
-Anestesiform: Generell
-Operationsberättelse: Cefuroxim iv peroperativt. Rak paramedian incision till höger om medellinjen. Ett borrhål. Spärrhake. Kryssformad durotomi. Kommer in på subduralhematom under högt tryck. Spolar med spolkateter och kompleterande handspol till klart utbyte. Tunnelerar ett subgalealt drän som fästs på sedvanligt sätt.  Syr sedan igen huden med inverterad enstaka Vicryl och fortlöpande Ethilon i hudplanet under bågående spol och med borrhålet som högsta punkt. 
-Post-operativa ordinationer: Suturtagning 12 dagar post-op. Subgalealt drän i 12-24 h. Ingen mer antibiotika.</t>
-  </si>
-  <si>
     <t>Daganteckning 24-01-25, kl 1514, Läk Sofia Johansson: 
 Patienten som under natten fick utrymt hö KSDH pga klinisk försämring. Bedömer pat på avd under dagen där patienten nu fått en klar klinisk förbättring. Rör armar och ben obehindrat i sängen. Klagar ej över huvudvärk. Ter sig adekvat i kontakten. Fortsatt något trött.
 Bed/åtgärd: Drar det subgaleala dränet under EM. Får bedömas av fysioterapeut och arbetsterapeut imorgon. Kan flyttas från vaksal till vanlig avdelsnignsplats.</t>
@@ -118,17 +108,6 @@
     <t>Daganteckning 24-01-26 kl 1132, Läk Sofia Johansson: 
 Bedömd av fysio och arbetsterapeut under förmiddagen. Ses fortsatt diskret nedsatt kraft i vänster arm och ben, men god gångförmåga. Fortsatt något trött men ej förvirrad. 
 Bedömning/åtgärd: Fortsatt träning på avd. Då patienten bor själv hemma ses indikation för vårdplanering då patienten kan behöva lite extra stöttning av hemtjänst initialt vid hemgång. Meddelar SSK att boka in vårdplanering med kommunen.</t>
-  </si>
-  <si>
-    <t>Daganteckning 24-01-27, kl 1523, Läk Torben Kristensen: 
-Patient som fått utrymt KSDH höger 24-01-24, se operationsberättelse och inskrivningsanteckning för bakgrund. Inväntar VPL. 
-Nu under dagen tilltagande trötthet och feber, temp 38,9 på morgonen. Patienten har inte orkat med träning med fysioterapeut. Hostat en del gulaktigt slem. 
-Objektivt: Krepitationer på lungerna basalt bilateralt. 
-RTG thorax: Infiltarationer i lungorna basalt bilateralt så som vid pneumoni. 
-Blodprov: CRP 60, LPK 15,6
-Urinsticka ua. 
-Mätvärden: BT 153/82, Saturation 95%, puls 94, temp 38,1
-Bed/åtgärd: Utvecklat lunginflammation. Insätter iv Benzylpenicillin 2 g x 3. Nya infektionsvärden imorgon. Blododling. Kontroller av mätvärden 4-5 ggr per dygn. Alvedon vb mot feber.</t>
   </si>
   <si>
     <t>Daganteckning 24-01-28, kl 0413, Läk Louise Carlsson: 
@@ -185,6 +164,117 @@
     <t>Slutanteckning</t>
   </si>
   <si>
+    <t>2024-01-23</t>
+  </si>
+  <si>
+    <t>2024-01-24</t>
+  </si>
+  <si>
+    <t>2024-01-25</t>
+  </si>
+  <si>
+    <t>2024-01-26</t>
+  </si>
+  <si>
+    <t>2024-01-27</t>
+  </si>
+  <si>
+    <t>2024-01-28</t>
+  </si>
+  <si>
+    <t>2024-01-29</t>
+  </si>
+  <si>
+    <t>2024-01-30</t>
+  </si>
+  <si>
+    <t>datum</t>
+  </si>
+  <si>
+    <t>anteckningstyp</t>
+  </si>
+  <si>
+    <t>Remiss (1/2)</t>
+  </si>
+  <si>
+    <t>Remiss (2/2)</t>
+  </si>
+  <si>
+    <t>Daganteckning (1/2)</t>
+  </si>
+  <si>
+    <t>Daganteckning (2/2)</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>2024-01-23: Extern kontakt rörande patient</t>
+  </si>
+  <si>
+    <t>2024-01-24: Inskrivningsanteckning</t>
+  </si>
+  <si>
+    <t>2024-01-24: Daganteckning</t>
+  </si>
+  <si>
+    <t>2024-01-24: Kommentar till undersökning</t>
+  </si>
+  <si>
+    <t>2024-01-25: Operationsberättelse</t>
+  </si>
+  <si>
+    <t>2024-01-25: Daganteckning</t>
+  </si>
+  <si>
+    <t>2024-01-26: Daganteckning</t>
+  </si>
+  <si>
+    <t>2024-01-27: Daganteckning</t>
+  </si>
+  <si>
+    <t>2024-01-28: Daganteckning (1/2)</t>
+  </si>
+  <si>
+    <t>2024-01-28: Daganteckning (2/2)</t>
+  </si>
+  <si>
+    <t>2024-01-29: Daganteckning</t>
+  </si>
+  <si>
+    <t>2024-01-30: Daganteckning</t>
+  </si>
+  <si>
+    <t>2024-01-30: Remiss (1/2)</t>
+  </si>
+  <si>
+    <t>2024-01-30: Remiss (2/2)</t>
+  </si>
+  <si>
+    <t>2024-01-30: Slutanteckning</t>
+  </si>
+  <si>
+    <t>Daganteckning 24-01-27, kl 1523, Läk Torben Kristensen: 
+Patient som fått utrymt KSDH höger 24-01-25, se operationsberättelse och inskrivningsanteckning för bakgrund. Inväntar VPL. 
+Nu under dagen tilltagande trötthet och feber, temp 38,9 på morgonen. Patienten har inte orkat med träning med fysioterapeut. Hostat en del gulaktigt slem. 
+Objektivt: Krepitationer på lungerna basalt bilateralt. 
+RTG thorax: Infiltarationer i lungorna basalt bilateralt så som vid pneumoni. 
+Blodprov: CRP 60, LPK 15,6
+Urinsticka ua. 
+Mätvärden: BT 153/82, Saturation 95%, puls 94, temp 38,1
+Bed/åtgärd: Utvecklat lunginflammation. Insätter iv Benzylpenicillin 2 g x 3. Nya infektionsvärden imorgon. Blododling. Kontroller av mätvärden 4-5 ggr per dygn. Alvedon vb mot feber.</t>
+  </si>
+  <si>
+    <t>Operationsberättelse 24-01-25, kl 0123, Läk Robin Gyllenskjöld: 
+Operationskod: AAD10 Utrymning av kroniskt subduralthematom höger
+Operatör: Robin Gyllenskjöld
+Operation: 5 Sahlgrenska
+Preoperativ bedömning: 63 årig man med HT, HL, rökare, som för ca 1 månad sedan ramlade och slog i huvudet. För ca 1 vecka sedan utvecklat smygande vä svaghet, haltande vä ben vid gång, balansbesvär, konstant tryckande huvudvärk VAS 6-7, förvirring. Inneliggande sedan 24-01-23. Under kvällen kliniskt försämrad, RLS 2-3, ytterligare vä svaghet. Bedöms indikation för akut utrymning. 
+Anestesiform: Generell
+Operationsberättelse: Cefuroxim iv peroperativt. Rak paramedian incision till höger om medellinjen. Ett borrhål. Spärrhake. Kryssformad durotomi. Kommer in på subduralhematom under högt tryck. Spolar med spolkateter och kompleterande handspol till klart utbyte. Tunnelerar ett subgalealt drän som fästs på sedvanligt sätt.  Syr sedan igen huden med inverterad enstaka Vicryl och fortlöpande Ethilon i hudplanet under bågående spol och med borrhålet som högsta punkt. 
+Post-operativa ordinationer: Suturtagning 12 dagar post-op. Subgalealt drän i 12-24 h. Ingen mer antibiotika.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Slutanteckning 24-01-30, Läk Torben Kristensen
 Diagnos: S065 Traumatiskt kroniskt subduralhematom 
 Bidiagnos: J189 Pneumoni, ospecificerad 
@@ -194,7 +284,7 @@
 Operatör: Robin Gyllenskjöld 24-01-25
 Vårdtid: 24-01-24 – 24-01-30
 Tidigare/Nuvarande sjukdomar: Tablettbehandlad hypertoni, hyperlipidemi, tidigare appendektomerad 2013, diskbråck lumbalt 2015 konservativt behandlat.
-Aktuellt: Falltrauma julafton 2023-01-24 där patienten slog i huvudet. Inkommer med 1 veckas anamnes på tilltagande svaghet vä sida samt dysartri och fascialispares. Noteras förvirrad och förändrad i kontakten enligt anhöriga. Huvudvärk frontalt och höger, VAS 6-7. 
+Aktuellt: Falltrauma julafton 2024-01-23 där patienten slog i huvudet. Inkommer med 1 veckas anamnes på tilltagande svaghet vä sida samt dysartri och fascialispares. Noteras förvirrad och förändrad i kontakten enligt anhöriga. Huvudvärk frontalt och höger, VAS 6-7. 
 Sammanfattning av vårdtid: Inkommer från SKaS 24-01-24. Noteras vä svaghet kraftgrad 4 till 4- vä arm och ben jmf med höger. Vä fascialispares och dysatri av mild typ. Påverkad balans och positiv rhomberg, släpar vä ben vid gång. CT hjärna från SKaS visade hö KSDH med begynnande masseffekt. Försämras kliniskt under kvällen 24/1, CT med utslätade fåror och tilltagande masseffekt, RLS 2-3, ytterligare vä svaghet. Tas till operation natten 25/1 för utrymning. Symptomen går i regress efter operation frånsett fortsatt diskret nedsatt kraft vä. Utvecklar under vårdtiden en pneumoni där patienten är syrgaskrävande, beh med iv Benzylpenicillin, därefter byte till Pip/taz. Efter antibiotikabyte klinisk förbättring. Blododling visar Klebsiella Pneumoniae. VPL där patienten beviljas hemtjänst x 2 dagligen. Skrivs ut med tabl antibiotika 30/1. Remiss till neurovårdsteam utfärdas, patienten önskar ej inneliggande rehab via Neurorehab Högsbo sjukhus. 
 Bedömning/åtgärd: Således 63 årig man med falltrauma under jul där patienten därefter utvecklar smygande vä svaghet, förvirring och huvudvärk. CT visar ett större KSDH höger som förklarar patientens symptom. Utryms 25/1 med god effekt. 
 Aktuell medicinlista: 
@@ -209,96 +299,6 @@
 Ingen planerad uppföljning via Neurokirurgen. 
 Sjukskrivning: 100% från 24-01-24 till 24-02-07
 Kopia: Sävedalen vårdcentral för kännedom. </t>
-  </si>
-  <si>
-    <t>2024-01-23</t>
-  </si>
-  <si>
-    <t>2024-01-24</t>
-  </si>
-  <si>
-    <t>2024-01-25</t>
-  </si>
-  <si>
-    <t>2024-01-26</t>
-  </si>
-  <si>
-    <t>2024-01-27</t>
-  </si>
-  <si>
-    <t>2024-01-28</t>
-  </si>
-  <si>
-    <t>2024-01-29</t>
-  </si>
-  <si>
-    <t>2024-01-30</t>
-  </si>
-  <si>
-    <t>datum</t>
-  </si>
-  <si>
-    <t>anteckningstyp</t>
-  </si>
-  <si>
-    <t>Remiss (1/2)</t>
-  </si>
-  <si>
-    <t>Remiss (2/2)</t>
-  </si>
-  <si>
-    <t>Daganteckning (1/2)</t>
-  </si>
-  <si>
-    <t>Daganteckning (2/2)</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>2024-01-23: Extern kontakt rörande patient</t>
-  </si>
-  <si>
-    <t>2024-01-24: Inskrivningsanteckning</t>
-  </si>
-  <si>
-    <t>2024-01-24: Daganteckning</t>
-  </si>
-  <si>
-    <t>2024-01-24: Kommentar till undersökning</t>
-  </si>
-  <si>
-    <t>2024-01-25: Operationsberättelse</t>
-  </si>
-  <si>
-    <t>2024-01-25: Daganteckning</t>
-  </si>
-  <si>
-    <t>2024-01-26: Daganteckning</t>
-  </si>
-  <si>
-    <t>2024-01-27: Daganteckning</t>
-  </si>
-  <si>
-    <t>2024-01-28: Daganteckning (1/2)</t>
-  </si>
-  <si>
-    <t>2024-01-28: Daganteckning (2/2)</t>
-  </si>
-  <si>
-    <t>2024-01-29: Daganteckning</t>
-  </si>
-  <si>
-    <t>2024-01-30: Daganteckning</t>
-  </si>
-  <si>
-    <t>2024-01-30: Remiss (1/2)</t>
-  </si>
-  <si>
-    <t>2024-01-30: Remiss (2/2)</t>
-  </si>
-  <si>
-    <t>2024-01-30: Slutanteckning</t>
   </si>
 </sst>
 </file>
@@ -711,9 +711,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E974"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -728,16 +728,16 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>1</v>
@@ -745,13 +745,13 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B2" s="6">
         <v>1234</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>2</v>
@@ -762,13 +762,13 @@
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B3" s="6">
         <v>1234</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>4</v>
@@ -779,13 +779,13 @@
     </row>
     <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B4" s="6">
         <v>1234</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>6</v>
@@ -796,13 +796,13 @@
     </row>
     <row r="5" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B5" s="6">
         <v>1234</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>8</v>
@@ -813,189 +813,189 @@
     </row>
     <row r="6" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B6" s="6">
         <v>1234</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B7" s="6">
         <v>1234</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B8" s="6">
         <v>1234</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B9" s="6">
         <v>1234</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B10" s="6">
         <v>1234</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B11" s="6">
         <v>1234</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B12" s="6">
         <v>1234</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B13" s="6">
         <v>1234</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B14" s="6">
         <v>1234</v>
       </c>
       <c r="C14" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>33</v>
-      </c>
       <c r="E14" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B15" s="6">
         <v>1234</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B16" s="6">
         <v>1234</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="3:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>